<commit_message>
use first subword token for model dist
</commit_message>
<xml_diff>
--- a/probing/file.xlsx
+++ b/probing/file.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -449,16 +449,6 @@
           <t>material</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>cooccur</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>coda</t>
-        </is>
-      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
@@ -466,27 +456,17 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>(0.5, 0.209, 49.3)</t>
+          <t>(0.475, 0.216, 41.8)</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>(0.497, 0.126, 70.7)</t>
+          <t>(0.482, 0.12, 64.3)</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>(0.415, 0.153, 57.4)</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>(0.014, 0.044, 3.6)</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>(0.462, 0.257, 40.2)</t>
+          <t>(0.419, 0.154, 55.3)</t>
         </is>
       </c>
     </row>
@@ -496,27 +476,17 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>(0.492, 0.196, 59.1)</t>
+          <t>(0.5, 0.198, 59.8)</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>(0.507, 0.166, 86.4)</t>
+          <t>(0.527, 0.1, 89.3)</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>(0.465, 0.135, 77.8)</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>(0.115, 0.084, 4.5)</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>(0.538, 0.248, 45.8)</t>
+          <t>(0.465, 0.137, 74.6)</t>
         </is>
       </c>
     </row>
@@ -526,27 +496,17 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>(0.54, 0.207, 58.7)</t>
+          <t>(0.537, 0.213, 57.7)</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>(0.521, 0.128, 73.6)</t>
+          <t>(0.514, 0.11, 74.3)</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>(0.462, 0.136, 76.8)</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>(0.112, 0.085, 9.3)</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>(0.575, 0.253, 58.9)</t>
+          <t>(0.46, 0.136, 74.6)</t>
         </is>
       </c>
     </row>
@@ -556,27 +516,17 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>(0.485, 0.194, 46.2)</t>
+          <t>(0.448, 0.198, 41.6)</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>(0.492, 0.14, 44.3)</t>
+          <t>(0.454, 0.124, 69.3)</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>(0.349, 0.21, 49.6)</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>(0.098, 0.06, 1.7)</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>(0.548, 0.23, 48.6)</t>
+          <t>(0.33, 0.155, 39.1)</t>
         </is>
       </c>
     </row>
@@ -586,27 +536,17 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>(0.243, 0.198, 16.6)</t>
+          <t>(0.202, 0.248, 13.4)</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>(0.427, 0.149, 24.3)</t>
+          <t>(0.298, 0.157, 13.6)</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>(0.373, 0.152, 45.1)</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>(0.075, 0.051, 1.0)</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>(0.302, 0.231, 35.5)</t>
+          <t>(0.25, 0.179, 27.8)</t>
         </is>
       </c>
     </row>
@@ -616,27 +556,17 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>(0.48, 0.205, 55.2)</t>
+          <t>(0.476, 0.209, 51.6)</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>(0.514, 0.134, 84.3)</t>
+          <t>(0.498, 0.131, 72.9)</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>(0.399, 0.151, 57.0)</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>(0.026, 0.023, 2.6)</t>
-        </is>
-      </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>(0.496, 0.233, 40.2)</t>
+          <t>(0.394, 0.16, 52.5)</t>
         </is>
       </c>
     </row>

</xml_diff>